<commit_message>
add few pages and comments, bugs fixed
</commit_message>
<xml_diff>
--- a/server/test/中期答辨分组.xlsx
+++ b/server/test/中期答辨分组.xlsx
@@ -5,6 +5,10 @@
   <sheets>
     <sheet name="第一组" sheetId="1" r:id="rId1"/>
     <sheet name="第二组" sheetId="2" r:id="rId2"/>
+    <sheet name="第三组" sheetId="3" r:id="rId3"/>
+    <sheet name="第四组" sheetId="4" r:id="rId4"/>
+    <sheet name="第五组" sheetId="5" r:id="rId5"/>
+    <sheet name="第六组" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -373,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -397,16 +401,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>1030513403</v>
+        <v>1030513218</v>
       </c>
       <c r="C2" t="str">
-        <v>陈亚楠</v>
+        <v>朱静</v>
       </c>
       <c r="D2" t="str">
-        <v>fagagaga</v>
+        <v>小区物业管理系统的设计与实现</v>
       </c>
       <c r="E2" t="str">
-        <v>张得天</v>
+        <v>蒋亦樟</v>
       </c>
     </row>
     <row r="3">
@@ -414,16 +418,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>1030513404</v>
+        <v>1030513431</v>
       </c>
       <c r="C3" t="str">
-        <v>丁钰莹</v>
+        <v>许嘉文</v>
       </c>
       <c r="D3" t="str">
-        <v>gaga</v>
+        <v>智能图像处理软件</v>
       </c>
       <c r="E3" t="str">
-        <v>张得天</v>
+        <v>邓赵红</v>
       </c>
     </row>
     <row r="4">
@@ -431,16 +435,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>1030513401</v>
+        <v>1030513207</v>
       </c>
       <c r="C4" t="str">
-        <v>蔡青</v>
+        <v>刘思燚</v>
       </c>
       <c r="D4" t="str">
-        <v>1233</v>
+        <v>网络在线人类特征识别软件开发</v>
       </c>
       <c r="E4" t="str">
-        <v>陈伟</v>
+        <v>邓赵红</v>
       </c>
     </row>
     <row r="5">
@@ -448,16 +452,186 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>1030513402</v>
+        <v>1030513130</v>
       </c>
       <c r="C5" t="str">
-        <v>陈慧敏</v>
+        <v>许鹏</v>
       </c>
       <c r="D5" t="str">
-        <v>qgagag</v>
+        <v>通用深度学习智能系统</v>
       </c>
       <c r="E5" t="str">
-        <v>陈伟</v>
+        <v>邓赵红</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1030513320</v>
+      </c>
+      <c r="C6" t="str">
+        <v>郑佳敏</v>
+      </c>
+      <c r="D6" t="str">
+        <v>跨域知识学习技术及其在医学成像处理中的应用</v>
+      </c>
+      <c r="E6" t="str">
+        <v>钱鹏江</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1030513420</v>
+      </c>
+      <c r="C7" t="str">
+        <v>杨艺</v>
+      </c>
+      <c r="D7" t="str">
+        <v>MapReduce分布式计算架构分析与实践</v>
+      </c>
+      <c r="E7" t="str">
+        <v>钱鹏江</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1030513104</v>
+      </c>
+      <c r="C8" t="str">
+        <v>郭苹苹</v>
+      </c>
+      <c r="D8" t="str">
+        <v>员工任务管理系统的设计与实现</v>
+      </c>
+      <c r="E8" t="str">
+        <v>蒋亦樟</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1030513208</v>
+      </c>
+      <c r="C9" t="str">
+        <v>卢虹羽</v>
+      </c>
+      <c r="D9" t="str">
+        <v>基于智能方法的癫痫脑电信号识别研究</v>
+      </c>
+      <c r="E9" t="str">
+        <v>蒋亦樟</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1030513421</v>
+      </c>
+      <c r="C10" t="str">
+        <v>余梦巧</v>
+      </c>
+      <c r="D10" t="str">
+        <v>基于模糊聚类的图像分割及其实现</v>
+      </c>
+      <c r="E10" t="str">
+        <v>王士同</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1030513315</v>
+      </c>
+      <c r="C11" t="str">
+        <v>汤希文</v>
+      </c>
+      <c r="D11" t="str">
+        <v>面向医学图像的图像融合技术研究</v>
+      </c>
+      <c r="E11" t="str">
+        <v>蒋亦樟</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>1030513205</v>
+      </c>
+      <c r="C12" t="str">
+        <v>刘孟楠</v>
+      </c>
+      <c r="D12" t="str">
+        <v>旅行社信息管理系统的设计与实现</v>
+      </c>
+      <c r="E12" t="str">
+        <v>蒋亦樟</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>1030513415</v>
+      </c>
+      <c r="C13" t="str">
+        <v>刘英姿</v>
+      </c>
+      <c r="D13" t="str">
+        <v>面向甲状腺癌诊断的智能识别技术探索</v>
+      </c>
+      <c r="E13" t="str">
+        <v>蒋亦樟</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>1030513111</v>
+      </c>
+      <c r="C14" t="str">
+        <v>龙仕清</v>
+      </c>
+      <c r="D14" t="str">
+        <v>安卓平台人类特征识别软件开发</v>
+      </c>
+      <c r="E14" t="str">
+        <v>邓赵红</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>1030513201</v>
+      </c>
+      <c r="C15" t="str">
+        <v>陈婷婷</v>
+      </c>
+      <c r="D15" t="str">
+        <v>移动端的益智游戏开发</v>
+      </c>
+      <c r="E15" t="str">
+        <v>邓赵红</v>
       </c>
     </row>
   </sheetData>
@@ -466,7 +640,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E25"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -490,16 +664,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>1030513405</v>
+        <v>1030513425</v>
       </c>
       <c r="C2" t="str">
-        <v>高斯理</v>
+        <v>郭震方</v>
       </c>
       <c r="D2" t="str">
-        <v>tqyqyq</v>
+        <v>云计算平台的运行与安全监控</v>
       </c>
       <c r="E2" t="str">
-        <v>狄岚</v>
+        <v>刘渊</v>
       </c>
     </row>
     <row r="3">
@@ -507,16 +681,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>1030513407</v>
+        <v>1030513426</v>
       </c>
       <c r="C3" t="str">
-        <v>洪嘉惠</v>
+        <v>蒋子才</v>
       </c>
       <c r="D3" t="str">
-        <v>gageqt</v>
+        <v>基于Javascript的虚拟实验开发</v>
       </c>
       <c r="E3" t="str">
-        <v>狄岚</v>
+        <v>刘渊</v>
       </c>
     </row>
     <row r="4">
@@ -524,16 +698,1714 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
+        <v>1030513304</v>
+      </c>
+      <c r="C4" t="str">
+        <v>贺怡</v>
+      </c>
+      <c r="D4" t="str">
+        <v>基于视频的目标计数与目标大小计算算法研究与实现</v>
+      </c>
+      <c r="E4" t="str">
+        <v>陈丽芳</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1030513132</v>
+      </c>
+      <c r="C5" t="str">
+        <v>张俊操</v>
+      </c>
+      <c r="D5" t="str">
+        <v>基于Jquery的Web前端应用开发</v>
+      </c>
+      <c r="E5" t="str">
+        <v>陈飞</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1030513231</v>
+      </c>
+      <c r="C6" t="str">
+        <v>许军</v>
+      </c>
+      <c r="D6" t="str">
+        <v>微信小程序开发</v>
+      </c>
+      <c r="E6" t="str">
+        <v>陈飞</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1030513409</v>
+      </c>
+      <c r="C7" t="str">
+        <v>黄心雨</v>
+      </c>
+      <c r="D7" t="str">
+        <v>无锡产业发展和人口成长趋势可视化调研</v>
+      </c>
+      <c r="E7" t="str">
+        <v>张军</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1030513407</v>
+      </c>
+      <c r="C8" t="str">
+        <v>洪嘉惠</v>
+      </c>
+      <c r="D8" t="str">
+        <v>基于压缩编码的数据隐藏算法的研究与实现</v>
+      </c>
+      <c r="E8" t="str">
+        <v>陈丽芳</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
         <v>1030513408</v>
       </c>
+      <c r="C9" t="str">
+        <v>华清沁</v>
+      </c>
+      <c r="D9" t="str">
+        <v>基于DirectX的全局光照算法SVO的框架软件开发</v>
+      </c>
+      <c r="E9" t="str">
+        <v>张军</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1030513233</v>
+      </c>
+      <c r="C10" t="str">
+        <v>郑雨杰</v>
+      </c>
+      <c r="D10" t="str">
+        <v>基于视频信息的测量与计算技术的研究</v>
+      </c>
+      <c r="E10" t="str">
+        <v>刘渊</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1030513310</v>
+      </c>
+      <c r="C11" t="str">
+        <v>马驰</v>
+      </c>
+      <c r="D11" t="str">
+        <v>社交网络的可视化研究的开发</v>
+      </c>
+      <c r="E11" t="str">
+        <v>刘渊</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>1030513212</v>
+      </c>
+      <c r="C12" t="str">
+        <v>夏雪娇</v>
+      </c>
+      <c r="D12" t="str">
+        <v>社交网络的可视化研究的开发</v>
+      </c>
+      <c r="E12" t="str">
+        <v>刘渊</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>1030513133</v>
+      </c>
+      <c r="C13" t="str">
+        <v>庄蒙周</v>
+      </c>
+      <c r="D13" t="str">
+        <v>基于真实云景照片的天空盒子纹理合成组件开发</v>
+      </c>
+      <c r="E13" t="str">
+        <v>张军</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>1030513402</v>
+      </c>
+      <c r="C14" t="str">
+        <v>陈慧敏</v>
+      </c>
+      <c r="D14" t="str">
+        <v>多维信息展示的课程辅助教学系统的研究与实现</v>
+      </c>
+      <c r="E14" t="str">
+        <v>陈丽芳</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>1030513120</v>
+      </c>
+      <c r="C15" t="str">
+        <v>于思涵</v>
+      </c>
+      <c r="D15" t="str">
+        <v>基于construct2的HTML5游戏开发</v>
+      </c>
+      <c r="E15" t="str">
+        <v>陈飞</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <v>1030513430</v>
+      </c>
+      <c r="C16" t="str">
+        <v>吴吉</v>
+      </c>
+      <c r="D16" t="str">
+        <v>本科毕业设计管理系统设计与实现</v>
+      </c>
+      <c r="E16" t="str">
+        <v>晏涛</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>1030513326</v>
+      </c>
+      <c r="C17" t="str">
+        <v>苏德志</v>
+      </c>
+      <c r="D17" t="str">
+        <v>立体图像匹配技术研究</v>
+      </c>
+      <c r="E17" t="str">
+        <v>晏涛</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <v>1030513203</v>
+      </c>
+      <c r="C18" t="str">
+        <v>李明泉</v>
+      </c>
+      <c r="D18" t="str">
+        <v>基于视频的目标识别与标记系统的研究与实现</v>
+      </c>
+      <c r="E18" t="str">
+        <v>陈丽芳</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>1030513107</v>
+      </c>
+      <c r="C19" t="str">
+        <v>黄敏园</v>
+      </c>
+      <c r="D19" t="str">
+        <v>cocos2d移动游戏开发</v>
+      </c>
+      <c r="E19" t="str">
+        <v>陈飞</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <v>1030513328</v>
+      </c>
+      <c r="C20" t="str">
+        <v>王家麟</v>
+      </c>
+      <c r="D20" t="str">
+        <v>多视点图像新视点生成技术研究</v>
+      </c>
+      <c r="E20" t="str">
+        <v>晏涛</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>1030513414</v>
+      </c>
+      <c r="C21" t="str">
+        <v>林瑞</v>
+      </c>
+      <c r="D21" t="str">
+        <v>基于图像的船型识别方法研究</v>
+      </c>
+      <c r="E21" t="str">
+        <v>晏涛</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <v>1030513131</v>
+      </c>
+      <c r="C22" t="str">
+        <v>姚铭</v>
+      </c>
+      <c r="D22" t="str">
+        <v>交互展陈（与艺术系老师合作）</v>
+      </c>
+      <c r="E22" t="str">
+        <v>陈丽芳</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="str">
+        <v>1030513433</v>
+      </c>
+      <c r="C23" t="str">
+        <v>朱聪聪</v>
+      </c>
+      <c r="D23" t="str">
+        <v>立体图像增强和自动编辑技术研究</v>
+      </c>
+      <c r="E23" t="str">
+        <v>晏涛</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="str">
+        <v>1030513324</v>
+      </c>
+      <c r="C24" t="str">
+        <v>邱志强</v>
+      </c>
+      <c r="D24" t="str">
+        <v>立体图像增强和自动编辑技术研究</v>
+      </c>
+      <c r="E24" t="str">
+        <v>晏涛</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="str">
+        <v>1030513126</v>
+      </c>
+      <c r="C25" t="str">
+        <v>沈苏明</v>
+      </c>
+      <c r="D25" t="str">
+        <v>基于ffmpeg的视频应用开发</v>
+      </c>
+      <c r="E25" t="str">
+        <v>陈飞</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E23"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>序号</v>
+      </c>
+      <c r="B1" t="str">
+        <v>学号</v>
+      </c>
+      <c r="C1" t="str">
+        <v>学生姓名</v>
+      </c>
+      <c r="D1" t="str">
+        <v>课题名</v>
+      </c>
+      <c r="E1" t="str">
+        <v>指导教师</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1030513204</v>
+      </c>
+      <c r="C2" t="str">
+        <v>李韵芝</v>
+      </c>
+      <c r="D2" t="str">
+        <v>基于微信的手游攻略平台设计</v>
+      </c>
+      <c r="E2" t="str">
+        <v>丁彦蕊</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1030513404</v>
+      </c>
+      <c r="C3" t="str">
+        <v>丁钰莹</v>
+      </c>
+      <c r="D3" t="str">
+        <v>基于matlab的气象台数据采集系统的设计与实现</v>
+      </c>
+      <c r="E3" t="str">
+        <v>丁彦蕊</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1030513409</v>
+      </c>
       <c r="C4" t="str">
+        <v>黄心雨</v>
+      </c>
+      <c r="D4" t="str">
+        <v>无锡产业发展和人口成长趋势可视化调研</v>
+      </c>
+      <c r="E4" t="str">
+        <v>张军</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1030513408</v>
+      </c>
+      <c r="C5" t="str">
         <v>华清沁</v>
       </c>
+      <c r="D5" t="str">
+        <v>基于DirectX的全局光照算法SVO的框架软件开发</v>
+      </c>
+      <c r="E5" t="str">
+        <v>张军</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1030513318</v>
+      </c>
+      <c r="C6" t="str">
+        <v>叶帼菁</v>
+      </c>
+      <c r="D6" t="str">
+        <v>大数据环境下的数据安全问题分析</v>
+      </c>
+      <c r="E6" t="str">
+        <v>丁彦蕊</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1030513119</v>
+      </c>
+      <c r="C7" t="str">
+        <v>姚陆吉</v>
+      </c>
+      <c r="D7" t="str">
+        <v>基于3ds max的城市小区动画漫游设计与实现</v>
+      </c>
+      <c r="E7" t="str">
+        <v>丁彦蕊</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1030513133</v>
+      </c>
+      <c r="C8" t="str">
+        <v>庄蒙周</v>
+      </c>
+      <c r="D8" t="str">
+        <v>基于真实云景照片的天空盒子纹理合成组件开发</v>
+      </c>
+      <c r="E8" t="str">
+        <v>张军</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1030513128</v>
+      </c>
+      <c r="C9" t="str">
+        <v>孙锐</v>
+      </c>
+      <c r="D9" t="str">
+        <v>图像特征与识别方法的研究与实现</v>
+      </c>
+      <c r="E9" t="str">
+        <v>陈秀宏</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1030513211</v>
+      </c>
+      <c r="C10" t="str">
+        <v>魏伊雪</v>
+      </c>
+      <c r="D10" t="str">
+        <v>基于MATLAB的图像处理应用系统设计与实现</v>
+      </c>
+      <c r="E10" t="str">
+        <v>狄岚</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1030513305</v>
+      </c>
+      <c r="C11" t="str">
+        <v>矫慧文</v>
+      </c>
+      <c r="D11" t="str">
+        <v>图像分割算法的研究与实现</v>
+      </c>
+      <c r="E11" t="str">
+        <v>狄岚</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>1030513405</v>
+      </c>
+      <c r="C12" t="str">
+        <v>高斯理</v>
+      </c>
+      <c r="D12" t="str">
+        <v>基于AR技术的某产品宣传</v>
+      </c>
+      <c r="E12" t="str">
+        <v>陈秀宏</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>1030513309</v>
+      </c>
+      <c r="C13" t="str">
+        <v>刘茜蓉</v>
+      </c>
+      <c r="D13" t="str">
+        <v>基于AR技术的某产品宣传</v>
+      </c>
+      <c r="E13" t="str">
+        <v>陈秀宏</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>1030512302</v>
+      </c>
+      <c r="C14" t="str">
+        <v>方旭</v>
+      </c>
+      <c r="D14" t="str">
+        <v>视频目标跟踪方法研究与实现</v>
+      </c>
+      <c r="E14" t="str">
+        <v>陈秀宏</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>1030513413</v>
+      </c>
+      <c r="C15" t="str">
+        <v>李越敏</v>
+      </c>
+      <c r="D15" t="str">
+        <v>基于Unity3D的VR项目设计与实现</v>
+      </c>
+      <c r="E15" t="str">
+        <v>丁彦蕊</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <v>1030513209</v>
+      </c>
+      <c r="C16" t="str">
+        <v>马莎莎</v>
+      </c>
+      <c r="D16" t="str">
+        <v>基于Unity的三维场景的交互设计与实现</v>
+      </c>
+      <c r="E16" t="str">
+        <v>狄岚</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>1030513307</v>
+      </c>
+      <c r="C17" t="str">
+        <v>李诗怡</v>
+      </c>
+      <c r="D17" t="str">
+        <v>基于Unity的三维场景的交互设计与实现</v>
+      </c>
+      <c r="E17" t="str">
+        <v>狄岚</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <v>1030513401</v>
+      </c>
+      <c r="C18" t="str">
+        <v>蔡青</v>
+      </c>
+      <c r="D18" t="str">
+        <v>基于VR技术的校园/景区漫游</v>
+      </c>
+      <c r="E18" t="str">
+        <v>陈秀宏</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>1030513108</v>
+      </c>
+      <c r="C19" t="str">
+        <v>李贝贝</v>
+      </c>
+      <c r="D19" t="str">
+        <v>基于MATLAB的人脸识别算法研究与实现</v>
+      </c>
+      <c r="E19" t="str">
+        <v>狄岚</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <v>1030513113</v>
+      </c>
+      <c r="C20" t="str">
+        <v>欧嘉琳</v>
+      </c>
+      <c r="D20" t="str">
+        <v>面向中学生的化学实验体验设计与实现</v>
+      </c>
+      <c r="E20" t="str">
+        <v>狄岚</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>1030513217</v>
+      </c>
+      <c r="C21" t="str">
+        <v>张筱雨</v>
+      </c>
+      <c r="D21" t="str">
+        <v>3D虚拟文物展示</v>
+      </c>
+      <c r="E21" t="str">
+        <v>陈秀宏</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <v>1030513118</v>
+      </c>
+      <c r="C22" t="str">
+        <v>薛丹彤</v>
+      </c>
+      <c r="D22" t="str">
+        <v>基于Matlab的语音信号的采集与分析</v>
+      </c>
+      <c r="E22" t="str">
+        <v>丁彦蕊</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="str">
+        <v>1030513102</v>
+      </c>
+      <c r="C23" t="str">
+        <v>杜亚男</v>
+      </c>
+      <c r="D23" t="str">
+        <v>基于人眼虹膜识别的安防系统开发</v>
+      </c>
+      <c r="E23" t="str">
+        <v>陈秀宏</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E17"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>序号</v>
+      </c>
+      <c r="B1" t="str">
+        <v>学号</v>
+      </c>
+      <c r="C1" t="str">
+        <v>学生姓名</v>
+      </c>
+      <c r="D1" t="str">
+        <v>课题名</v>
+      </c>
+      <c r="E1" t="str">
+        <v>指导教师</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1030513429</v>
+      </c>
+      <c r="C2" t="str">
+        <v>王伟林</v>
+      </c>
+      <c r="D2" t="str">
+        <v>基于监控视频的会展人流特征分析及可视化</v>
+      </c>
+      <c r="E2" t="str">
+        <v>谢振平</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1030513303</v>
+      </c>
+      <c r="C3" t="str">
+        <v>陈晓琪</v>
+      </c>
+      <c r="D3" t="str">
+        <v>大规模网络关系图的可视化研究</v>
+      </c>
+      <c r="E3" t="str">
+        <v>谢振平</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1030513219</v>
+      </c>
+      <c r="C4" t="str">
+        <v>朱彦超</v>
+      </c>
       <c r="D4" t="str">
-        <v>gageqt</v>
+        <v>大规模网络关系图的可视化研究</v>
       </c>
       <c r="E4" t="str">
-        <v>狄岚</v>
+        <v>谢振平</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1030513101</v>
+      </c>
+      <c r="C5" t="str">
+        <v>陈梅婕</v>
+      </c>
+      <c r="D5" t="str">
+        <v>大数据行为特征智能挖掘技术研究</v>
+      </c>
+      <c r="E5" t="str">
+        <v>谢振平</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1030513428</v>
+      </c>
+      <c r="C6" t="str">
+        <v>王涛</v>
+      </c>
+      <c r="D6" t="str">
+        <v>食品安全动态数据的自动化采集与应用</v>
+      </c>
+      <c r="E6" t="str">
+        <v>谢振平</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1030513431</v>
+      </c>
+      <c r="C7" t="str">
+        <v>许嘉文</v>
+      </c>
+      <c r="D7" t="str">
+        <v>智能图像处理软件</v>
+      </c>
+      <c r="E7" t="str">
+        <v>邓赵红</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1030513111</v>
+      </c>
+      <c r="C8" t="str">
+        <v>龙仕清</v>
+      </c>
+      <c r="D8" t="str">
+        <v>安卓平台人类特征识别软件开发</v>
+      </c>
+      <c r="E8" t="str">
+        <v>邓赵红</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1030513213</v>
+      </c>
+      <c r="C9" t="str">
+        <v>徐慧敏</v>
+      </c>
+      <c r="D9" t="str">
+        <v>基于用户行为的电影推荐系统构建</v>
+      </c>
+      <c r="E9" t="str">
+        <v>夏鸿斌</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1030513319</v>
+      </c>
+      <c r="C10" t="str">
+        <v>赵欢</v>
+      </c>
+      <c r="D10" t="str">
+        <v>基于html5的移动应用开发</v>
+      </c>
+      <c r="E10" t="str">
+        <v>夏鸿斌</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1030513314</v>
+      </c>
+      <c r="C11" t="str">
+        <v>史罗琼</v>
+      </c>
+      <c r="D11" t="str">
+        <v>与艺术性合作：基于unity交互引擎的数字艺术表现(章立)</v>
+      </c>
+      <c r="E11" t="str">
+        <v>夏鸿斌</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>1030513117</v>
+      </c>
+      <c r="C12" t="str">
+        <v>吴慧中</v>
+      </c>
+      <c r="D12" t="str">
+        <v>与艺术性合作：基于unity交互引擎的数字艺术表现(章立)</v>
+      </c>
+      <c r="E12" t="str">
+        <v>夏鸿斌</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>1030513207</v>
+      </c>
+      <c r="C13" t="str">
+        <v>刘思燚</v>
+      </c>
+      <c r="D13" t="str">
+        <v>网络在线人类特征识别软件开发</v>
+      </c>
+      <c r="E13" t="str">
+        <v>邓赵红</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>1030513201</v>
+      </c>
+      <c r="C14" t="str">
+        <v>陈婷婷</v>
+      </c>
+      <c r="D14" t="str">
+        <v>移动端的益智游戏开发</v>
+      </c>
+      <c r="E14" t="str">
+        <v>邓赵红</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>1030513410</v>
+      </c>
+      <c r="C15" t="str">
+        <v>贾玉珍</v>
+      </c>
+      <c r="D15" t="str">
+        <v>基于LEAP Motion的手势识别技术构建新闻头条浏览系统</v>
+      </c>
+      <c r="E15" t="str">
+        <v>夏鸿斌</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <v>1030513121</v>
+      </c>
+      <c r="C16" t="str">
+        <v>陈衍瑜</v>
+      </c>
+      <c r="D16" t="str">
+        <v>基于开源架构的微博情感倾向性分析</v>
+      </c>
+      <c r="E16" t="str">
+        <v>夏鸿斌</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>1030513130</v>
+      </c>
+      <c r="C17" t="str">
+        <v>许鹏</v>
+      </c>
+      <c r="D17" t="str">
+        <v>通用深度学习智能系统</v>
+      </c>
+      <c r="E17" t="str">
+        <v>邓赵红</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E22"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>序号</v>
+      </c>
+      <c r="B1" t="str">
+        <v>学号</v>
+      </c>
+      <c r="C1" t="str">
+        <v>学生姓名</v>
+      </c>
+      <c r="D1" t="str">
+        <v>课题名</v>
+      </c>
+      <c r="E1" t="str">
+        <v>指导教师</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1030513306</v>
+      </c>
+      <c r="C2" t="str">
+        <v>李佳慧</v>
+      </c>
+      <c r="D2" t="str">
+        <v>基于移动互联模式改进非遗馆展项的系统开发与应用</v>
+      </c>
+      <c r="E2" t="str">
+        <v>孟磊</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1030513333</v>
+      </c>
+      <c r="C3" t="str">
+        <v>余帆</v>
+      </c>
+      <c r="D3" t="str">
+        <v>基于Arduino的三维动画动态投影</v>
+      </c>
+      <c r="E3" t="str">
+        <v>赵燕</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1030513322</v>
+      </c>
+      <c r="C4" t="str">
+        <v>郭晟</v>
+      </c>
+      <c r="D4" t="str">
+        <v>中国大陆新闻传播学学术文献数据库建设</v>
+      </c>
+      <c r="E4" t="str">
+        <v>黄秋儒</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1030513109</v>
+      </c>
+      <c r="C5" t="str">
+        <v>李丹</v>
+      </c>
+      <c r="D5" t="str">
+        <v>亚投行的国际舆情监测及数据可视化分析</v>
+      </c>
+      <c r="E5" t="str">
+        <v>吴锋</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1030513127</v>
+      </c>
+      <c r="C6" t="str">
+        <v>史忠源</v>
+      </c>
+      <c r="D6" t="str">
+        <v>境外反华群体性事件舆情监测及可视化研究（可小组执行）</v>
+      </c>
+      <c r="E6" t="str">
+        <v>吴锋</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1030513423</v>
+      </c>
+      <c r="C7" t="str">
+        <v>曹钰</v>
+      </c>
+      <c r="D7" t="str">
+        <v>绘本的动态化数字展示</v>
+      </c>
+      <c r="E7" t="str">
+        <v>赵燕</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1030513416</v>
+      </c>
+      <c r="C8" t="str">
+        <v>彭开云</v>
+      </c>
+      <c r="D8" t="str">
+        <v>AR技术在购物环境应用下的交互设计</v>
+      </c>
+      <c r="E8" t="str">
+        <v>赵燕</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1030513220</v>
+      </c>
+      <c r="C9" t="str">
+        <v>朱雨婷</v>
+      </c>
+      <c r="D9" t="str">
+        <v>基于虚拟现实技术的地方非遗保护程序设计</v>
+      </c>
+      <c r="E9" t="str">
+        <v>黄秋儒</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1030513216</v>
+      </c>
+      <c r="C10" t="str">
+        <v>张倩倩</v>
+      </c>
+      <c r="D10" t="str">
+        <v>服务设计思维下非遗馆数字化展项体验优化路径研究</v>
+      </c>
+      <c r="E10" t="str">
+        <v>孟磊</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1030513106</v>
+      </c>
+      <c r="C11" t="str">
+        <v>贺东莉</v>
+      </c>
+      <c r="D11" t="str">
+        <v>医学教学视频中的3D转制应用与设计</v>
+      </c>
+      <c r="E11" t="str">
+        <v>黄秋儒</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>1030513105</v>
+      </c>
+      <c r="C12" t="str">
+        <v>郭越</v>
+      </c>
+      <c r="D12" t="str">
+        <v>境外媒体对中国高铁的报道监测及数据可视化分析</v>
+      </c>
+      <c r="E12" t="str">
+        <v>吴锋</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>1030513110</v>
+      </c>
+      <c r="C13" t="str">
+        <v>刘逸虹</v>
+      </c>
+      <c r="D13" t="str">
+        <v>“中国制造”在国外媒体的呈现框架及数据可视化分析</v>
+      </c>
+      <c r="E13" t="str">
+        <v>吴锋</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>1030513202</v>
+      </c>
+      <c r="C14" t="str">
+        <v>杜倩倩</v>
+      </c>
+      <c r="D14" t="str">
+        <v>后工业语境下的数字技术与文化遗产整合应用方法探析</v>
+      </c>
+      <c r="E14" t="str">
+        <v>孟磊</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>1030513210</v>
+      </c>
+      <c r="C15" t="str">
+        <v>田馨月</v>
+      </c>
+      <c r="D15" t="str">
+        <v>无锡地区非遗的数字化保护与传承（殷俊）</v>
+      </c>
+      <c r="E15" t="str">
+        <v>黄秋儒</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <v>1030513206</v>
+      </c>
+      <c r="C16" t="str">
+        <v>刘楠</v>
+      </c>
+      <c r="D16" t="str">
+        <v>非遗语境下的博物馆交互性展示设计</v>
+      </c>
+      <c r="E16" t="str">
+        <v>黄秋儒</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>1030513311</v>
+      </c>
+      <c r="C17" t="str">
+        <v>马鲁昕</v>
+      </c>
+      <c r="D17" t="str">
+        <v>基于视频特效的影视短片制作</v>
+      </c>
+      <c r="E17" t="str">
+        <v>黄秋儒</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <v>1030513308</v>
+      </c>
+      <c r="C18" t="str">
+        <v>梁雪晴</v>
+      </c>
+      <c r="D18" t="str">
+        <v>基于情感体验的交互设计</v>
+      </c>
+      <c r="E18" t="str">
+        <v>赵燕</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>1030513215</v>
+      </c>
+      <c r="C19" t="str">
+        <v>湛倩倩</v>
+      </c>
+      <c r="D19" t="str">
+        <v>中国大陆突发群体性事件数据库建设</v>
+      </c>
+      <c r="E19" t="str">
+        <v>吴锋</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <v>1030513228</v>
+      </c>
+      <c r="C20" t="str">
+        <v>谢尚逊</v>
+      </c>
+      <c r="D20" t="str">
+        <v>面向文化场馆的分布式互动展示系统开发</v>
+      </c>
+      <c r="E20" t="str">
+        <v>孟磊</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>1030513331</v>
+      </c>
+      <c r="C21" t="str">
+        <v>吴若宇</v>
+      </c>
+      <c r="D21" t="str">
+        <v>三维动画设计</v>
+      </c>
+      <c r="E21" t="str">
+        <v>赵燕</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <v>1030513316</v>
+      </c>
+      <c r="C22" t="str">
+        <v>王君临</v>
+      </c>
+      <c r="D22" t="str">
+        <v>基于VR技术的交互设计</v>
+      </c>
+      <c r="E22" t="str">
+        <v>赵燕</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>序号</v>
+      </c>
+      <c r="B1" t="str">
+        <v>学号</v>
+      </c>
+      <c r="C1" t="str">
+        <v>学生姓名</v>
+      </c>
+      <c r="D1" t="str">
+        <v>课题名</v>
+      </c>
+      <c r="E1" t="str">
+        <v>指导教师</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>1030513321</v>
+      </c>
+      <c r="C2" t="str">
+        <v>葛亮</v>
+      </c>
+      <c r="D2" t="str">
+        <v>欺诈短信的数据挖掘</v>
+      </c>
+      <c r="E2" t="str">
+        <v>张得天</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1030513125</v>
+      </c>
+      <c r="C3" t="str">
+        <v>刘俊</v>
+      </c>
+      <c r="D3" t="str">
+        <v>魔方拼图</v>
+      </c>
+      <c r="E3" t="str">
+        <v>陈伟</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1030513313</v>
+      </c>
+      <c r="C4" t="str">
+        <v>倪晓琪</v>
+      </c>
+      <c r="D4" t="str">
+        <v>单色透明shader&amp;标准镜面高光shader</v>
+      </c>
+      <c r="E4" t="str">
+        <v>林意</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1030513103</v>
+      </c>
+      <c r="C5" t="str">
+        <v>甘姣姣</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Web前端开发</v>
+      </c>
+      <c r="E5" t="str">
+        <v>张得天</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1030513403</v>
+      </c>
+      <c r="C6" t="str">
+        <v>陈亚楠</v>
+      </c>
+      <c r="D6" t="str">
+        <v>从无序到有序：点列迭代中的神奇</v>
+      </c>
+      <c r="E6" t="str">
+        <v>陈伟</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1030513317</v>
+      </c>
+      <c r="C7" t="str">
+        <v>杨悦</v>
+      </c>
+      <c r="D7" t="str">
+        <v>像素的颜色：从算法到艺术</v>
+      </c>
+      <c r="E7" t="str">
+        <v>陈伟</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>1030513221</v>
+      </c>
+      <c r="C8" t="str">
+        <v>戴杰</v>
+      </c>
+      <c r="D8" t="str">
+        <v>OpenCV哈夫变换线圆检测实现</v>
+      </c>
+      <c r="E8" t="str">
+        <v>林意</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1030513129</v>
+      </c>
+      <c r="C9" t="str">
+        <v>王斌</v>
+      </c>
+      <c r="D9" t="str">
+        <v>基于企业数据的爬虫</v>
+      </c>
+      <c r="E9" t="str">
+        <v>张得天</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1030513112</v>
+      </c>
+      <c r="C10" t="str">
+        <v>毛姝婧</v>
+      </c>
+      <c r="D10" t="str">
+        <v>微信公众号前端开发</v>
+      </c>
+      <c r="E10" t="str">
+        <v>张得天</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1030513223</v>
+      </c>
+      <c r="C11" t="str">
+        <v>李振明</v>
+      </c>
+      <c r="D11" t="str">
+        <v>OpenCV仿射变换与SURF特征点描述</v>
+      </c>
+      <c r="E11" t="str">
+        <v>林意</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>1030513124</v>
+      </c>
+      <c r="C12" t="str">
+        <v>刘家旺</v>
+      </c>
+      <c r="D12" t="str">
+        <v>OpenCV边缘检测之比较</v>
+      </c>
+      <c r="E12" t="str">
+        <v>林意</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>1030513332</v>
+      </c>
+      <c r="C13" t="str">
+        <v>肖山民</v>
+      </c>
+      <c r="D13" t="str">
+        <v>垂直爬虫开发</v>
+      </c>
+      <c r="E13" t="str">
+        <v>张得天</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>1030513412</v>
+      </c>
+      <c r="C14" t="str">
+        <v>李诗芸</v>
+      </c>
+      <c r="D14" t="str">
+        <v>基于Unity3D屏幕特效实现</v>
+      </c>
+      <c r="E14" t="str">
+        <v>林意</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>1030513325</v>
+      </c>
+      <c r="C15" t="str">
+        <v>宋旭飞</v>
+      </c>
+      <c r="D15" t="str">
+        <v>基于微信公众号的搜索平台设计与实现</v>
+      </c>
+      <c r="E15" t="str">
+        <v>张得天</v>
       </c>
     </row>
   </sheetData>

</xml_diff>